<commit_message>
accomodation request upload and map with student
</commit_message>
<xml_diff>
--- a/Licenta/wwwroot/UploadIdCards/IdCards.xlsx
+++ b/Licenta/wwwroot/UploadIdCards/IdCards.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="27">
   <si>
     <t>Birthdate</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>TC 419786</t>
+  </si>
+  <si>
+    <t>SPCLEP Tulcea</t>
+  </si>
+  <si>
+    <t>Str. Sabinelor</t>
   </si>
 </sst>
 </file>
@@ -414,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2755,7 +2764,7 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>544194</v>
+        <v>456382</v>
       </c>
       <c r="D81" t="s">
         <v>23</v>
@@ -2773,6 +2782,35 @@
         <v>21</v>
       </c>
       <c r="I81" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>35765</v>
+      </c>
+      <c r="B82" t="s">
+        <v>9</v>
+      </c>
+      <c r="C82" t="s">
+        <v>24</v>
+      </c>
+      <c r="D82" t="s">
+        <v>25</v>
+      </c>
+      <c r="E82" s="1">
+        <v>42539</v>
+      </c>
+      <c r="F82" t="s">
+        <v>20</v>
+      </c>
+      <c r="G82" t="s">
+        <v>20</v>
+      </c>
+      <c r="H82" t="s">
+        <v>26</v>
+      </c>
+      <c r="I82" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>